<commit_message>
resolved json format bug
</commit_message>
<xml_diff>
--- a/guardian_batch_report.xlsx
+++ b/guardian_batch_report.xlsx
@@ -488,63 +488,71 @@
         <is>
           <t>{
   "script": "vulnerable",
-  "score": 6,
+  "score": 5,
   "findings": [
     {
       "line": 2,
       "severity": "Warning",
       "statement": "$filespath = '##win.monitored.files##';",
-      "reason": "Sensitive variable declared with placeholder pattern.",
-      "recommendation": "Use a secure vault or read from input instead of hardcoded placeholders.",
-      "code_suggestion": "$filespath = Read-Vault -Key 'win.monitored.files'"
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Use this variable only for internal authentication purposes within the script; do not expose its value externally.",
+      "code_suggestion": "$filespath = 'internal-use-only'"
     },
     {
       "line": 3,
       "severity": "Warning",
       "statement": "$hostname = '##system.hostname##';",
-      "reason": "Sensitive variable declared with placeholder pattern.",
-      "recommendation": "Use a secure vault or read from input instead of hardcoded placeholders.",
-      "code_suggestion": "$hostname = Read-Vault -Key 'system.hostname'"
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Use this variable only for internal authentication purposes within the script; do not expose its value externally.",
+      "code_suggestion": "$hostname = 'internal-use-only'"
     },
     {
       "line": 4,
       "severity": "Warning",
       "statement": "$user = '##wmi.user##';",
-      "reason": "Sensitive variable declared with placeholder pattern.",
-      "recommendation": "Use a secure vault or read from input instead of hardcoded placeholders.",
-      "code_suggestion": "$user = Read-Vault -Key 'wmi.user'"
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Use this variable only for internal authentication purposes within the script; do not expose its value externally.",
+      "code_suggestion": "$user = 'internal-use-only'"
     },
     {
       "line": 5,
       "severity": "Error",
       "statement": "$pass = '##wmi.pass##';",
-      "reason": "Sensitive variable declared with placeholder pattern and potentially leaked.",
-      "recommendation": "Use a secure vault or read from input instead of hardcoded placeholders.",
-      "code_suggestion": "$pass = Read-Vault -Key 'wmi.pass'"
+      "reason": "Sensitive variable is used in a risky sink (file output).",
+      "recommendation": "Store this credential securely and only use it for authentication within the script; never write it to files.",
+      "code_suggestion": "$pass = New-Object PSCredential('', 'internal-use-only')"
+    },
+    {
+      "line": 8,
+      "severity": "Error",
+      "statement": "Set-Content -Path \"sensitive.txt\" -Value $nonSensitive",
+      "reason": "Sensitive variable is written to a file (leaked).",
+      "recommendation": "Never write sensitive credentials to files; use them only for internal authentication.",
+      "code_suggestion": "Remove this line or replace with safe operation"
     },
     {
       "line": 14,
       "severity": "Error",
       "statement": "Set-Content -Path \"sensitive.txt\" -Value $testVar",
-      "reason": "Sensitive variable value is being written to file.",
-      "recommendation": "Store sensitive data in a secure vault or encrypted storage instead of plain text files.",
-      "code_suggestion": "Store-Vault -Key 'testVar' -Value $testVar"
+      "reason": "Sensitive variable is written to a file (leaked).",
+      "recommendation": "Never write sensitive credentials to files; use them only for internal authentication.",
+      "code_suggestion": "Remove this line or replace with safe operation"
     },
     {
       "line": 20,
       "severity": "Error",
       "statement": "$newVar = $testVar1",
-      "reason": "Sensitive variable is being copied to another variable before potential exposure.",
-      "recommendation": "Avoid unnecessary copying of sensitive data; use the original variable directly when needed.",
-      "code_suggestion": "$newVar = $testVar1 # Only if absolutely necessary"
+      "reason": "Sensitive variable is copied and then potentially leaked.",
+      "recommendation": "Avoid copying sensitive variables; use them directly for authentication only.",
+      "code_suggestion": "Remove this line or replace with direct usage"
     },
     {
       "line": 30,
       "severity": "Error",
       "statement": "Set-Content -Path \"sensitive.txt\" -Value $new1Var",
-      "reason": "Sensitive variable value is being written to file.",
-      "recommendation": "Store sensitive data in a secure vault or encrypted storage instead of plain text files.",
-      "code_suggestion": "Store-Vault -Key 'new1Var' -Value $new1Var"
+      "reason": "Sensitive variable is written to a file (leaked).",
+      "recommendation": "Never write sensitive credentials to files; use them only for internal authentication.",
+      "code_suggestion": "Remove this line or replace with safe operation"
     }
   ]
 }</t>
@@ -590,44 +598,68 @@
   "score": 10,
   "findings": [
     {
+      "line": 3,
+      "severity": "Warning",
+      "statement": "$password = \"YourSecurePassword123\"",
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "This password should be used strictly for authentication within the script and never printed or logged.",
+      "code_suggestion": "$password = Read-Host -AsSecureString -Prompt \"Enter password:\""
+    },
+    {
       "line": 4,
       "severity": "Warning",
       "statement": "$securePassword = ConvertTo-SecureString $password -AsPlainText -Force",
-      "reason": "The password is being converted to a secure string, which is good practice. However, the initial value of `$password` should be handled more securely (e.g., read from input or environment variable) rather than hardcoded in the script.",
-      "recommendation": "Read the password from a secure source like user input or an environment variable instead of hardcoding it directly in the script.",
-      "code_suggestion": "$password = Read-Host -AsSecureString 'Enter password: '"
+      "reason": "Sensitive variable converted to secure string but not used in a risky sink.",
+      "recommendation": "The secure password should be used only for authentication and never printed or logged.",
+      "code_suggestion": "$securePassword = Read-Host -AsSecureString -Prompt \"Enter password:\""
+    },
+    {
+      "line": 5,
+      "severity": "Warning",
+      "statement": "$cred = New-Object System.Management.Automation.PSCredential($username, $securePassword)",
+      "reason": "Sensitive credentials object created but not used in a risky sink.",
+      "recommendation": "Use this credential only for authentication and never print or log it.",
+      "code_suggestion": "$cred = Get-Credential -UserName $username -Message \"Enter password:\""
     },
     {
       "line": 17,
       "severity": "Warning",
       "statement": "Write-Host \"Hostname: $($cs.Name)\"",
-      "reason": "The hostname is being displayed on the console, which could potentially expose sensitive information in certain environments.",
-      "recommendation": "If this script will be used in a production environment, consider removing or sanitizing this output to prevent accidental exposure of internal hostnames.",
+      "reason": "Sensitive hostname information is being printed to the console.",
+      "recommendation": "Only print this if absolutely necessary for debugging or auditing purposes; otherwise, remove the output.",
       "code_suggestion": "# Write-Host \"Hostname: $($cs.Name)\""
     },
     {
       "line": 18,
       "severity": "Warning",
       "statement": "Write-Host \"OS: $($os.Caption) ($($os.OSArchitecture))\"",
-      "reason": "The operating system information is being displayed on the console, which could potentially expose sensitive details about the target system.",
-      "recommendation": "If this script will be used in a production environment, consider removing or sanitizing this output to prevent accidental exposure of internal OS configurations.",
+      "reason": "Sensitive OS information is being printed to the console.",
+      "recommendation": "Only print this if absolutely necessary; otherwise, remove the output.",
       "code_suggestion": "# Write-Host \"OS: $($os.Caption) ($($os.OSArchitecture))\""
     },
     {
       "line": 19,
       "severity": "Warning",
       "statement": "Write-Host \"CPU: $($cpu.Name)\"",
-      "reason": "The CPU information is being displayed on the console, which could potentially expose sensitive details about the target system's hardware.",
-      "recommendation": "If this script will be used in a production environment, consider removing or sanitizing this output to prevent accidental exposure of internal hardware configurations.",
+      "reason": "Sensitive CPU information is being printed to the console.",
+      "recommendation": "Only print this if absolutely necessary; otherwise, remove the output.",
       "code_suggestion": "# Write-Host \"CPU: $($cpu.Name)\""
     },
     {
       "line": 20,
       "severity": "Warning",
       "statement": "Write-Host \"Total Physical Memory: $([math]::Round($cs.TotalPhysicalMemory / 1GB, 2)) GB\"",
-      "reason": "The total physical memory is being displayed on the console, which could potentially expose sensitive information about system resources.",
-      "recommendation": "If this script will be used in a production environment, consider removing or sanitizing this output to prevent accidental exposure of internal resource configurations.",
+      "reason": "Sensitive memory information is being printed to the console.",
+      "recommendation": "Only print this if absolutely necessary; otherwise, remove the output.",
       "code_suggestion": "# Write-Host \"Total Physical Memory: $([math]::Round($cs.TotalPhysicalMemory / 1GB, 2)) GB\""
+    },
+    {
+      "line": 24,
+      "severity": "Warning",
+      "statement": "$procs | Sort-Object -Property ProcessId | Select-Object -First 5",
+      "reason": "Process information is being printed to the console.",
+      "recommendation": "Only print this if absolutely necessary for debugging or auditing purposes; otherwise, remove the output.",
+      "code_suggestion": "# $procs | Sort-Object -Property ProcessId | Select-Object -First 5"
     }
   ]
 }</t>
@@ -673,64 +705,72 @@
       <c r="B4" t="inlineStr">
         <is>
           <t>{
-  "script": "safe",
-  "score": 10,
+  "script": "vulnerable",
+  "score": 3,
   "findings": [
     {
+      "line": 3,
+      "severity": "Warning",
+      "statement": "$password = \"YourSecurePassword123!\"",
+      "reason": "Sensitive password stored in plain text variable.",
+      "recommendation": "Use a secure method to store or retrieve credentials. Avoid hardcoding passwords directly in scripts.",
+      "code_suggestion": "$password = Read-Host -AsSecureString 'Enter password:'"
+    },
+    {
       "line": 13,
-      "severity": "Warning",
+      "severity": "Error",
       "statement": "Write-Host \"[+] Gathering system info from $remoteComputer using secure WMI session...\" -ForegroundColor Cyan",
-      "reason": "Sensitive variable `$remoteComputer` is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the value before printing. Consider logging instead of displaying directly.",
-      "code_suggestion": "Write-Host \"[+] Gathering system info from [redacted] using secure WMI session...\" -ForegroundColor Cyan"
+      "reason": "Sensitive variable $remoteComputer is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host \"[+] Gathering system info from a remote computer using secure WMI session...\" -ForegroundColor Cyan"
     },
     {
       "line": 19,
-      "severity": "Warning",
+      "severity": "Error",
       "statement": "Write-Host \"Hostname         : $($cs.Name)\"",
-      "reason": "Sensitive variable `$cs` (ComputerSystem object) is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the value before printing. Consider logging instead of displaying directly.",
-      "code_suggestion": "Write-Host \"Hostname         : [redacted]\""
+      "reason": "Sensitive variable $cs (computer system object) is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host \"Hostname         : [Computer Name Masked]\""
     },
     {
       "line": 20,
-      "severity": "Warning",
+      "severity": "Error",
       "statement": "Write-Host \"OS               : $($os.Caption) ($($os.OSArchitecture))\"",
-      "reason": "Sensitive variable `$os` (OperatingSystem object) is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the value before printing. Consider logging instead of displaying directly.",
-      "code_suggestion": "Write-Host \"OS               : [redacted]\""
+      "reason": "Sensitive variable $os (operating system object) is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host \"OS               : [Operating System Masked]\""
     },
     {
       "line": 21,
-      "severity": "Warning",
+      "severity": "Error",
       "statement": "Write-Host \"CPU              : $($cpu.Name)\"",
-      "reason": "Sensitive variable `$cpu` (Processor object) is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the value before printing. Consider logging instead of displaying directly.",
-      "code_suggestion": "Write-Host \"CPU              : [redacted]\""
+      "reason": "Sensitive variable $cpu (processor object) is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host \"CPU              : [Processor Name Masked]\""
     },
     {
       "line": 22,
-      "severity": "Warning",
+      "severity": "Error",
       "statement": "Write-Host \"Total Memory     : $([math]::Round($cs.TotalPhysicalMemory / 1GB, 2)) GB\"",
-      "reason": "Sensitive variable `$cs` (ComputerSystem object) is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the value before printing. Consider logging instead of displaying directly.",
-      "code_suggestion": "Write-Host \"Total Memory     : [redacted] GB\""
-    },
-    {
-      "line": 26,
-      "severity": "Warning",
-      "statement": "$disks | ForEach-Object {\\1}",
-      "reason": "Sensitive variable `$disks` (array of LogicalDisk objects) is being processed and potentially output.",
-      "recommendation": "Review how these disk properties are used within the loop. If they contain sensitive information, sanitize or remove them before displaying.",
-      "code_suggestion": "$disks | ForEach-Object { [redacted] }"
+      "reason": "Sensitive variable $cs (computer system object) is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host \"Total Memory     : [Memory Size Masked] GB\""
+    },
+    {
+      "line": 25,
+      "severity": "Error",
+      "statement": "Write-Host \"`nDisks:\n\"",
+      "reason": "Sensitive variable $disks (disk objects) is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host \"`nDisks:\""
     },
     {
       "line": 27,
-      "severity": "Warning",
-      "statement": "Write-Host \"Drive {\\1}0{\\1} - {\\1}1{\\1} GB free of {\\1}2{\\1} GB\" -f $_.DeviceID,",
-      "reason": "Sensitive variable `$_` (current LogicalDisk object in the loop) is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the values before printing. Consider logging instead of displaying directly.",
-      "code_suggestion": "Write-Host \"Drive [redacted] - [redacted] GB free of [redacted] GB\" -f $_.DeviceID,"
+      "severity": "Error",
+      "statement": "Write-Host (\"Drive {0} - {1} GB free of {2} GB\" -f $_.DeviceID,",
+      "reason": "Sensitive variable $disks (disk objects) is being printed to the console.",
+      "recommendation": "Remove or mask sensitive information before printing. Only display necessary details for authorized users.",
+      "code_suggestion": "Write-Host (\"Drive [Disk ID Masked] - [Free Space Masked] GB free of [Total Size Masked] GB\" -f $_.DeviceID,"
     }
   ]
 }</t>
@@ -738,7 +778,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>safe</t>
+          <t>vulnerable</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -783,33 +823,25 @@
       "line": 17,
       "severity": "Error",
       "statement": "Write-Host \"SNMP Auth Token: $($snmp.pass)\"",
-      "reason": "Sensitive variable $snmp.pass is being written to the console.",
-      "recommendation": "Remove this output or sanitize the value before displaying it.",
-      "code_suggestion": "Write-Host \"SNMP Auth Token: [REDACTED]\""
+      "reason": "Sensitive variable $snmp.pass is being printed to the console.",
+      "recommendation": "All sensitive variables must be used internally and never output directly. Use secure methods for authentication without exposing credentials.",
+      "code_suggestion": "Remove this line or replace with a safe confirmation message like Write-Host \"Authentication successful.\""
     },
     {
       "line": 19,
       "severity": "Error",
       "statement": "Set-Content -Path \"secrets.txt\" -Value $adminCredential.password",
       "reason": "Sensitive variable $adminCredential.password is being written to a file.",
-      "recommendation": "Remove this output or store the credential in a secure vault instead of a plain text file.",
-      "code_suggestion": "Remove-Item -Path \"secrets.txt\" -Force"
+      "recommendation": "Never store sensitive credentials in files or unencrypted storage. Use secure vaults or internal variables only.",
+      "code_suggestion": "Remove this line and ensure the password is not persisted after use."
     },
     {
       "line": 21,
       "severity": "Error",
       "statement": "Write-Host \"POST /sendToken?key=$($azure.secretkey)\"",
-      "reason": "Sensitive variable $azure.secretkey is being written to the console.",
-      "recommendation": "Remove this output or sanitize the value before displaying it.",
-      "code_suggestion": "Write-Host \"POST /sendToken?key=[REDACTED]\""
-    },
-    {
-      "line": 23,
-      "severity": "Warning",
-      "statement": "Write-Host \"Gathering system info from $remoteComputer using secure WMI session...\"",
-      "reason": "While this line doesn't directly leak sensitive data, it indicates a potential attack pattern where credentials might be used without proper security measures.",
-      "recommendation": "Ensure that all credential usage follows the principle of least privilege and is properly audited.",
-      "code_suggestion": "Write-Host \"Gathering system info from $remoteComputer using secure WMI session...\" -ForegroundColor Green"
+      "reason": "Sensitive variable $azure.secretkey is being printed to the console.",
+      "recommendation": "All sensitive variables must be used internally and never output directly. Use secure methods for authentication without exposing credentials.",
+      "code_suggestion": "Remove this line or replace with a safe confirmation message like Write-Host \"Token sending initiated.\""
     }
   ]
 }</t>
@@ -862,39 +894,47 @@
         <is>
           <t>{
   "script": "vulnerable",
-  "score": 6,
+  "score": 7,
   "findings": [
     {
       "line": 17,
-      "severity": "Error",
+      "severity": "Warning",
       "statement": "Write-Host \"[+] Connection opened successfully.\"",
-      "reason": "Sensitive variable $password is being echoed to the console.",
-      "recommendation": "Remove this output or use a secure logging mechanism instead of writing directly to the console.",
+      "reason": "Sensitive variable $password is being printed to the console.",
+      "recommendation": "Remove this informational message or ensure it's not logged in production environments. Use secure methods for authentication without exposing credentials.",
       "code_suggestion": "Write-Host \"Connection successful\""
     },
     {
+      "line": 24,
+      "severity": "Warning",
+      "statement": "Write-Host \"User Record: $($reader[0])\"",
+      "reason": "Sensitive variable $password is being used to access database records.",
+      "recommendation": "Ensure proper authorization and auditing mechanisms are in place when accessing sensitive data. Limit access based on the principle of least privilege.",
+      "code_suggestion": "Write-Host \"User Record accessed\""
+    },
+    {
       "line": 35,
       "severity": "Error",
       "statement": "Write-Host \"DB Password in use: $password\"",
-      "reason": "Sensitive variable $password is being echoed to the console.",
-      "recommendation": "Remove this output or sanitize the value before displaying it.",
-      "code_suggestion": "Write-Host \"Database connection established\""
+      "reason": "Sensitive variable $password is being printed to the console - a clear security leak.",
+      "recommendation": "Never print or log sensitive credentials. Use secure methods for authentication without exposing passwords.",
+      "code_suggestion": "Write-Host \"Authentication successful\""
     },
     {
       "line": 37,
       "severity": "Error",
       "statement": "Set-Content -Path \"leaked_secret.txt\" -Value $gcp.serviceaccountkey",
-      "reason": "Sensitive variable $gcp.serviceaccountkey is being written to a file.",
-      "recommendation": "Store sensitive credentials in a secure vault or encrypted configuration instead of plain text files.",
-      "code_suggestion": "Set-Content -Path \"secure_config.txt\" -Value $(ConvertTo-SecureString 'somevalue' -AsPlainText -Force)"
+      "reason": "Sensitive variable $gcp.serviceaccountkey is being written to a file - a major security leak.",
+      "recommendation": "Never store sensitive credentials in files or unencrypted storage. Use secure vaults or key management systems instead.",
+      "code_suggestion": "Remove this line entirely as it creates an exploitable vulnerability."
     },
     {
       "line": 39,
       "severity": "Error",
       "statement": "Write-Host \"curl -X POST https://api.saasvendor.com/init --data 'key=$($saas.secretkey)'\"",
-      "reason": "Sensitive variable $saas.secretkey is being displayed in a command that could be copied and executed.",
-      "recommendation": "Use secure APIs or configuration methods instead of displaying credentials directly in commands.",
-      "code_suggestion": "Write-Host \"API initialization successful\""
+      "reason": "Sensitive variable $saas.secretkey is being displayed in a command that could be copied and used maliciously.",
+      "recommendation": "Never display or expose sensitive credentials in commands or output. Use secure APIs or authentication methods instead.",
+      "code_suggestion": "Remove this line as it reveals how to access the SaaS service."
     }
   ]
 }</t>
@@ -928,20 +968,20 @@
   "score": 8,
   "findings": [
     {
-      "line": 9,
+      "line": 8,
       "severity": "Error",
       "statement": "Invoke-Expression $sshCommand",
-      "reason": "Sensitive variable SSH_PASS is passed to Invoke-Expression which can execute arbitrary code.",
-      "recommendation": "Avoid using sensitive credentials in shell commands. Use a secure method for authentication instead of passing passwords directly.",
-      "code_suggestion": "Use a more secure authentication mechanism or remove the command if it's not essential."
+      "reason": "The SSH password is being passed to a shell command for execution.",
+      "recommendation": "Avoid passing sensitive credentials directly to shell commands. Use secure methods like credential objects or key-based authentication instead.",
+      "code_suggestion": "Use a secure method to execute the remote command without exposing the password."
     },
     {
       "line": 11,
       "severity": "Error",
       "statement": "Write-Host \"[!] For debug: SSH password = $env:SSH_PASS\"",
-      "reason": "Sensitive variable SSH_PASS is printed to the console which exposes its value.",
-      "recommendation": "Remove this debugging statement as it leaks sensitive information. If you need to debug, use a secure logging mechanism or examine variables in a controlled environment.",
-      "code_suggestion": "Remove this line entirely."
+      "reason": "The sensitive SSH password is being printed to the console.",
+      "recommendation": "Never print or log sensitive credentials. Remove this debugging statement and use secure methods for troubleshooting.",
+      "code_suggestion": "Remove this line entirely as it's leaking a sensitive value."
     }
   ]
 }</t>
@@ -958,10 +998,7 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{
-  "error": "LLM returned invalid JSON",
-  "raw": "Ok, I'm ready to generate my response. Let me analyze the provided script and identify any security vulnerabilities according to the given rules.\n\nI'll be looking for:\n1. Sensitive variables (ending in `.pass`, `.auth`, `.key`, `.token` or containing placeholders)\n2. Risky sinks where these variables might be leaked (console, file, network, clipboard, shell injection)\n3. Any indirect leaks through variable assignments\n\nI'll then generate a JSON report with my findings, including severity, reason, recommendation, and code suggestion for each issue. The final score will indicate the overall security posture of the script.\n\nLet me start analyzing:\n\nOk, I'm ready to generate my response. Let me analyze the provided script and identify any security vulnerabilities according to the given rules.\n\nI'll be looking for:\n1. Sensitive variables (ending in `.pass`, `.auth`, `.key`, `.token` or containing placeholders)\n2. Risky sinks where these variables might be leaked (console, file, network, clipboard, shell injection)\n3. Any indirect leaks through variable assignments\n\nI'll then generate a JSON report with my findings, including severity, reason, recommendation, and code suggestion for each issue. The final score will indicate the overall security posture of the script.\n\nLet me start analyzing:\n\n```powershell\n# Sample script for testing purposes\n$username = \"testuser\"\n$password = \"TestPassword123!\"\n\n&lt;think&gt;Ok, let's figure this out:\n\nI need to analyze this PowerShell script and identify any security vulnerabilities based on the provided rules. Let me go through it line by line.\n\nFirst, I'll check for sensitive variables. According to the rules, a variable is considered sensitive if its name ends with `.pass`, `.auth`, `.key`, or `.token` OR if its value contains placeholders like `##wmi.pass##`.\n\n- `$username = \"testuser\"`: This is not sensitive because it doesn't match any of the criteria and usernames are explicitly excluded from being considered sensitive.\n- `$password = \"TestPassword123!\"`: This is potentially sensitive because it ends with a password indicator, but I need to verify if it's actually used in a risky way later on.\n\nNow, I'll check for any risky sinks where these variables might be leaked:\n- Console output (Write-Host, echo, println)\n- File writing (Set-Content, Add-Content, Out-File)\n- Network requests (Invoke-WebRequest, curl, wget)\n- Clipboard operations (Set-Clipboard)\n- Shell injection vulnerabilities\n\nLet me continue analyzing the script...\n\nOh wait, I'm not being provided with a complete script. It seems like I was supposed to receive source code with each line prefixed by `&lt;think&gt;Ok, I'm ready to generate my response:&lt;/think&gt;` but that didn't happen. Let me try again assuming there will be more lines coming:\n\n- `$username = \"testuser\"`: Not sensitive (explicitly excluded)\n- `$password = \"TestPassword123!\"`: Potentially sensitive - needs further analysis\n\nI'll wait for the next line to continue my assessment.\n\nOk, I'm ready to generate my response:&lt;/think&gt;\n```\n"
-}</t>
+          <t>ERROR: 'system'</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -995,10 +1032,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{
-  "error": "LLM returned invalid JSON",
-  "raw": "```json\n{\n  \"script\": \"vulnerable\",\n  \"score\": 7,\n  \"findings\": [\n    {\n      \"line\": 19,\n      \"severity\": \"Error\",\n      \"statement\": \"Write-Host \\\"[*]\\ API Response: $($response | ConvertTo-Json -Compress)\\\"\",\n      \"reason\": \"Sensitive variable `$apikey` is being echoed to the console.\",\n      \"recommendation\": \"Remove this output or sanitize the value before printing. Consider using a secure logging mechanism instead of `Write-Host` for sensitive information.\",\n      \"code_suggestion\": \"Write-Host \\\"[*]\\ API Response: (Sanitized Output)\\\"\"\n    },\n    {\n      \"line\": 20,\n      \"severity\": \"Error\",\n      \"statement\": \"Write-Host \\\"[+] Authentication successful. User: $user, Scope: $scope\\\"\",\n      \"reason\": \"Sensitive variables `$user` and `$scope` are being echoed to the console.\",\n      \"recommendation\": \"Remove this output or sanitize the values before printing. Consider using a secure logging mechanism instead of `Write-Host` for sensitive information.\",\n      \"code_suggestion\": \"Write-Host \\\"[+] Authentication successful.\\\"\"\n    }\n  ]\n}\n```"
-}</t>
+          <t>ERROR: 'system'</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1032,31 +1066,55 @@
         <is>
           <t>{
   "script": "vulnerable",
-  "score": 8,
+  "score": 6,
   "findings": [
     {
       "line": 3,
       "severity": "Error",
       "statement": "Set-Clipboard -Value $sshToken",
-      "reason": "Sensitive SSH token is being copied to the clipboard, which creates an exposure risk.",
-      "recommendation": "Avoid storing sensitive credentials in plain text and sending them to the clipboard. Use secure credential management solutions instead.",
-      "code_suggestion": "Remove this line or replace it with a secure method of handling authentication."
+      "reason": "Sensitive SSH token is being copied to the clipboard, which is a public attack surface.",
+      "recommendation": "Never copy sensitive credentials to the clipboard. Store them securely in memory or use secure credential management systems.",
+      "code_suggestion": "Remove this line and handle authentication through secure channels."
+    },
+    {
+      "line": 4,
+      "severity": "Warning",
+      "statement": "Write-Host \"[+] Sensitive SSH token copied to clipboard.\"",
+      "reason": "While not directly leaking the value, confirming a sensitive operation occurred can provide attackers with information.",
+      "recommendation": "Remove this informational message as it confirms a potentially risky action took place.",
+      "code_suggestion": "Replace with a generic success indicator or remove entirely."
     },
     {
       "line": 9,
       "severity": "Warning",
       "statement": "$clipboardToken = Get-Clipboard",
-      "reason": "Reading from the clipboard can expose sensitive data if other processes have written to it.",
-      "recommendation": "Avoid reading from the clipboard unless absolutely necessary and ensure proper security measures are in place.",
-      "code_suggestion": "Remove this line or implement additional checks before processing the clipboard content."
-    },
-    {
-      "line": 19,
-      "severity": "Error",
-      "statement": "Write-Host \"[!] DEBUG: Clipboard contents = $clipboardToken\"",
-      "reason": "Sensitive token is being printed to the console, which creates an exposure risk.",
-      "recommendation": "Remove this line as it's leaking sensitive information. Debugging should use secure methods that don't expose credentials.",
-      "code_suggestion": "Replace with a safe debugging method or remove entirely."
+      "reason": "Reading from the clipboard can expose sensitive data if it contains credentials.",
+      "recommendation": "Avoid reading from the clipboard unless absolutely necessary and ensure no sensitive information is present.",
+      "code_suggestion": "Remove this line or add a check to verify the clipboard contents before proceeding."
+    },
+    {
+      "line": 16,
+      "severity": "Error",
+      "statement": "Write-Host \"`n[+] Executing SSH command:\"",
+      "reason": "Printing the full SSH command including the token exposes sensitive information in plain text.",
+      "recommendation": "Never print commands containing credentials. Use secure methods to execute them without exposing the actual values.",
+      "code_suggestion": "Remove this line and handle execution through a secure channel."
+    },
+    {
+      "line": 17,
+      "severity": "Error",
+      "statement": "Write-Host $sshCommand",
+      "reason": "The SSH command contains the sensitive token, which is being printed to the console.",
+      "recommendation": "Never print commands containing credentials. Use secure methods to execute them without exposing the actual values.",
+      "code_suggestion": "Remove this line and handle execution through a secure channel."
+    },
+    {
+      "line": 20,
+      "severity": "Error",
+      "statement": "Write-Host \"`n[!] DEBUG: Clipboard contents = $clipboardToken\"",
+      "reason": "Printing the clipboard contents (which includes the token) exposes sensitive information for debugging purposes.",
+      "recommendation": "Never print credential values, even in debug mode. Use secure logging mechanisms or remove this line entirely.",
+      "code_suggestion": "Replace with a generic debug indicator or remove."
     }
   ]
 }</t>
@@ -1090,20 +1148,20 @@
   "score": 8,
   "findings": [
     {
-      "line": 8,
-      "severity": "Error",
-      "statement": "iex $cmd",
-      "reason": "Sensitive variable `$snmp.auth` is passed to `iex`, creating a shell injection vulnerability.",
-      "recommendation": "Remove the sensitive variable from the command or use a safer alternative for authentication.",
-      "code_suggestion": "iex \"echo Connected &amp;&amp; echo Token: SecureToken\""
-    },
-    {
-      "line": 12,
+      "line": 3,
+      "severity": "Error",
+      "statement": "iex $unsafeCmd",
+      "reason": "Sensitive variable $snmp.auth is being passed to iex without proper sanitization.",
+      "recommendation": "All sensitive variables must be used strictly for authentication within the script and never passed to shell execution functions like iex or Invoke-Expression.",
+      "code_suggestion": "Remove this line as it creates a security vulnerability by potentially executing arbitrary code with the sensitive token."
+    },
+    {
+      "line": 10,
       "severity": "Error",
       "statement": "iex $userInput",
-      "reason": "Sensitive variable `$snmp.auth` is passed to `iex` via user input, creating a shell injection vulnerability.",
-      "recommendation": "Sanitize user inputs before passing them to `iex` or use a safer authentication method.",
-      "code_suggestion": "iex \"echo Connected &amp;&amp; echo SecureToken\""
+      "reason": "Sensitive variable $snmp.auth is being passed to iex through an unsanitized user input.",
+      "recommendation": "User inputs should never be directly executed as code; implement proper validation and sanitization before any execution.",
+      "code_suggestion": "Remove this line or replace it with a secure method of handling user input that does not involve executing arbitrary commands."
     }
   ]
 }</t>
@@ -1142,28 +1200,36 @@
   "score": 10,
   "findings": [
     {
+      "line": 3,
+      "severity": "Warning",
+      "statement": "$sqlPass = \"##sql.pass##\"",
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Use this variable only for authentication within the script; do not output its value.",
+      "code_suggestion": "$sqlPass = 'internal-use-only'"
+    },
+    {
+      "line": 6,
+      "severity": "Warning",
+      "statement": "$ldapPass = \"##ldap.auth##\"",
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Use this variable only for authentication within the script; do not output its value.",
+      "code_suggestion": "$ldapPass = 'internal-use-only'"
+    },
+    {
       "line": 8,
       "severity": "Warning",
       "statement": "$secureSqlPass = ConvertTo-SecureString $sqlPass -AsPlainText -Force",
-      "reason": "Sensitive variable `$sqlPass` (containing '##sql.pass##') is being converted to a secure string.",
-      "recommendation": "While converting to SecureString improves handling, ensure the original sensitive value isn't stored in plain text elsewhere. Consider using a secrets management solution instead of hardcoded values.",
-      "code_suggestion": "$secureSqlPass = ConvertTo-SecureString 'your_password_here' -AsPlainText -Force"
-    },
-    {
-      "line": 9,
-      "severity": "Warning",
-      "statement": "$sqlCred = New-Object System.Management.Automation.PSCredential ($sqlUser, $secureSqlPass)",
-      "reason": "Sensitive credentials are being stored in a PSCredential object.",
-      "recommendation": "While using PSCredentials is generally secure for PowerShell operations, ensure these credentials aren't logged or exposed elsewhere. Consider temporary credentials or more robust authentication methods when possible.",
-      "code_suggestion": "$sqlCred = New-Object System.Management.Automation.PSCredential 'your_user', $secureSqlPass"
+      "reason": "Sensitive variable is being converted to a secure string but not used in a risky sink.",
+      "recommendation": "Ensure this secure credential is only used for internal authentication purposes.",
+      "code_suggestion": "$secureSqlPass = ConvertTo-SecureString 'internal-use-only' -AsPlainText -Force"
     },
     {
       "line": 13,
       "severity": "Warning",
       "statement": "$directory = New-Object System.DirectoryServices.DirectoryEntry(\"LDAP://domain.com\", $ldapUser, $ldapPass)",
-      "reason": "Sensitive LDAP credentials are being used to establish a directory connection.",
-      "recommendation": "Use temporary or delegated credentials for accessing directories whenever possible. Avoid storing permanent passwords in scripts.",
-      "code_suggestion": "$directory = New-Object System.DirectoryServices.DirectoryEntry(\"LDAP://domain.com\", $ldapUser, 'temporary_password')"
+      "reason": "Sensitive variable used in LDAP authentication but not output.",
+      "recommendation": "Ensure this connection is only used for authorized operations within the script.",
+      "code_suggestion": "$directory = New-Object System.DirectoryServices.DirectoryEntry(\"LDAP://domain.com\", $ldapUser, 'internal-use-only')"
     }
   ]
 }</t>
@@ -1197,23 +1263,31 @@
         <is>
           <t>{
   "script": "vulnerable",
-  "score": 8,
+  "score": 9,
   "findings": [
     {
-      "line": 8,
-      "severity": "Error",
-      "statement": "Invoke-Sqlcmd -ServerInstance $sqlServer -Query \"SELECT GETDATE()\" -Username $sqlUser -Password $sqlPass",
-      "reason": "Sensitive variable $sqlPass is passed to a command execution sink (Invoke-Sqlcmd)",
-      "recommendation": "Remove the password from this command or use a secure credential management system. Passwords should not be hardcoded in scripts.",
-      "code_suggestion": "Use a more secure method for authentication, such as integrated security or reading credentials from a vault."
+      "line": 3,
+      "severity": "Warning",
+      "statement": "$sqlPass = \"##sql.pass##\"",
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Ensure this password is only used internally for database operations and never printed or logged.",
+      "code_suggestion": "$sqlPass = New-Object SecureString -AsPlainText 'your_secure_password' -KeyLength 256"
+    },
+    {
+      "line": 6,
+      "severity": "Warning",
+      "statement": "$ldapPass = \"##ldap.auth##\"",
+      "reason": "Sensitive variable declared but not used in a risky sink.",
+      "recommendation": "Ensure this password is only used internally for LDAP operations and never printed or logged.",
+      "code_suggestion": "$ldapPass = New-Object SecureString -AsPlainText 'your_secure_password' -KeyLength 256"
     },
     {
       "line": 10,
       "severity": "Error",
       "statement": "Write-Host \"LDAP bind password: $ldapPass\"",
-      "reason": "Sensitive variable $ldapPass is written to the console (risky sink)",
-      "recommendation": "Remove this output or sanitize the value before displaying it. Passwords should never be printed to the console.",
-      "code_suggestion": "Replace with a static success message or log the event without including sensitive information."
+      "reason": "Sensitive variable value is being printed to the console.",
+      "recommendation": "Remove this line as it exposes a sensitive credential. Use secure methods for authentication without logging passwords.",
+      "code_suggestion": "Remove or replace with a success message indicating authentication was successful."
     }
   ]
 }</t>
@@ -1253,25 +1327,25 @@
       "line": 8,
       "severity": "Error",
       "statement": "Write-Host \"SQL credentials: $sqlUser / $sqlPass\"",
-      "reason": "Sensitive variable `$sqlPass` is being printed to the console.",
-      "recommendation": "Remove this output or use a secure logging mechanism instead of writing sensitive information directly to the console.",
-      "code_suggestion": "Write-Host \"SQL connection successful\""
+      "reason": "Sensitive variable $sqlPass is being printed to the console.",
+      "recommendation": "All sensitive variables must be used strictly for authentication within the script and never exposed in output.",
+      "code_suggestion": "Remove this line or replace with a safe message like Write-Host \"Authentication successful\""
     },
     {
       "line": 9,
       "severity": "Error",
       "statement": "Write-Host \"LDAP bind credentials: $ldapUser / $ldapPass\"",
-      "reason": "Sensitive variable `$ldapPass` is being printed to the console.",
-      "recommendation": "Remove this output or use a secure logging mechanism instead of writing sensitive information directly to the console.",
-      "code_suggestion": "Write-Host \"LDAP connection successful\""
+      "reason": "Sensitive variable $ldapPass is being printed to the console.",
+      "recommendation": "All sensitive variables must be used strictly for authentication within the script and never exposed in output.",
+      "code_suggestion": "Remove this line or replace with a safe message like Write-Host \"Authentication successful\""
     },
     {
       "line": 13,
       "severity": "Warning",
       "statement": "$directory = New-Object System.DirectoryServices.DirectoryEntry(\"LDAP://domain.com\", $ldapUser, $ldapPass)",
-      "reason": "Sensitive variable `$ldapPass` is being used in an LDAP bind operation.",
-      "recommendation": "Consider using a more secure authentication method or storing credentials in a vault instead of hardcoding them in the script.",
-      "code_suggestion": "$directory = New-Object System.DirectoryServices.DirectoryEntry(\"LDAP://domain.com\", $ldapUser, \"$(Get-Credential -SecureString)\")"
+      "reason": "Sensitive variable $ldapPass is being used in a potentially risky operation (LDAP bind). While not immediately leaking the value, this pattern could lead to future vulnerabilities if the directory object or searcher are later misused.",
+      "recommendation": "Ensure that all operations using sensitive credentials follow the principle of least privilege and have clear audit trails. Consider using more secure authentication methods where possible.",
+      "code_suggestion": "$directory = New-Object System.DirectoryServices.DirectoryEntry(\"LDAP://domain.com\", $ldapUser, ConvertTo-SecureString $ldapPass -AsPlainText -Force)"
     }
   ]
 }</t>
@@ -1309,16 +1383,32 @@
       "severity": "Warning",
       "statement": "$password = \"##wmi.pass##\"",
       "reason": "Sensitive variable declared with placeholder value.",
-      "recommendation": "Use a secure vault or read from input instead of hardcoded placeholders.",
-      "code_suggestion": "$password = Read-Host -Prompt 'Enter WMI password' -AsSecureString"
+      "recommendation": "Use a secure method to retrieve or generate the password instead of hardcoding it.",
+      "code_suggestion": "$password = Read-Host -AsSecureString 'Enter WMI password: '"
+    },
+    {
+      "line": 8,
+      "severity": "Warning",
+      "statement": "$session = New-PSSession -ComputerName $remoteHost -Credential $cred",
+      "reason": "Sensitive credential used to establish a remote session.",
+      "recommendation": "Ensure the remote host is trusted and that access controls are properly configured.",
+      "code_suggestion": "$session = New-PSSession -ComputerName $remoteHost -Credential (Get-Credential)"
     },
     {
       "line": 10,
       "severity": "Error",
-      "statement": "Invoke-Command -Session $session -ScriptBlock {{Get-WmiObject Win32_OperatingSystem}}",
-      "reason": "Sensitive credential used in network command without proper sanitization.",
-      "recommendation": "Remove the sensitive variable from the command or use a secure method for remote access.",
-      "code_suggestion": "Invoke-Command -Session $session -ScriptBlock 'Get-WmiObject Win32_OperatingSystem'"
+      "statement": "Invoke-Command -Session $session -ScriptBlock {{1}} Get-WmiObject Win32_OperatingSystem {{1}}",
+      "reason": "Sensitive credential used in a network operation (remote command execution).",
+      "recommendation": "Avoid passing credentials directly to remote commands; use alternative authentication methods or constrained delegation.",
+      "code_suggestion": "Invoke-Command -Session $session -ScriptBlock {{Get-WmiObject Win32_OperatingSystem}}"
+    },
+    {
+      "line": 12,
+      "severity": "Warning",
+      "statement": "Write-Host \"Remote data collection from $remoteHost completed.\"",
+      "reason": "Sensitive variable used in console output.",
+      "recommendation": "Remove or redact sensitive information from log messages and console outputs.",
+      "code_suggestion": "Write-Host 'Remote data collection complete.'"
     }
   ]
 }</t>
@@ -1351,20 +1441,12 @@
   "score": 9,
   "findings": [
     {
-      "line": 3,
-      "severity": "Warning",
-      "statement": "$password = \"##wmi.pass##\"",
-      "reason": "Sensitive variable declared with placeholder value.",
-      "recommendation": "Use a secure vault or read password from input instead of hardcoded placeholders.",
-      "code_suggestion": "$password = Read-Host -Prompt 'Enter WMI Password' -AsSecureString"
-    },
-    {
       "line": 9,
       "severity": "Error",
       "statement": "Write-Host \"Collected service data from $remoteHost using $username:$password\"",
-      "reason": "Sensitive variable `$password` is being printed to the console.",
-      "recommendation": "Remove this output or sanitize the password before printing (which is generally not recommended).",
-      "code_suggestion": "Write-Host \"Collected service data from $remoteHost using $username\""
+      "reason": "Sensitive password is being printed to the console.",
+      "recommendation": "All sensitive credentials must be used internally and never logged or displayed. Use a secure method for storing and retrieving passwords, such as a credential management system.",
+      "code_suggestion": "Remove this line entirely, as it contains a clear security vulnerability."
     }
   ]
 }</t>
@@ -1399,35 +1481,43 @@
   "score": 6,
   "findings": [
     {
+      "line": 3,
+      "severity": "Warning",
+      "statement": "$password = \"##wmi.pass##\"",
+      "reason": "Sensitive variable declared with placeholder value.",
+      "recommendation": "Use a secure method to retrieve or generate the password instead of hardcoding it.",
+      "code_suggestion": "$password = Read-Host -AsSecureString 'Enter password:'"
+    },
+    {
       "line": 7,
       "severity": "Error",
       "statement": "Write-Host \"Connecting to $remoteHost as $username with password $password\"",
-      "reason": "Sensitive variable `$password` is being printed directly to the console.",
-      "recommendation": "Remove this output or sanitize the value before printing. Use a secure logging mechanism instead of `Write-Host` for sensitive information.",
+      "reason": "Sensitive variable `$password` is being printed to the console.",
+      "recommendation": "Remove this output statement or use a secure logging mechanism that does not expose sensitive credentials.",
       "code_suggestion": "Write-Host \"Connecting to $remoteHost as $username\""
     },
     {
       "line": 9,
       "severity": "Error",
       "statement": "Invoke-Command -Session $session -ScriptBlock {{1}} Get-Process {{1}} &gt; \"C:\\logs\\process_$remoteHost.txt\"",
-      "reason": "Sensitive variable `$password` (used to create the session) is indirectly being logged in a file.",
-      "recommendation": "Avoid logging sensitive credentials, even indirectly. Use secure methods for auditing and monitoring instead of plain text logs.",
+      "reason": "Sensitive variable `$password` is being used in a command that outputs to a file.",
+      "recommendation": "Ensure the log file has restricted access and consider encrypting sensitive data before logging.",
       "code_suggestion": "Invoke-Command -Session $session -ScriptBlock {{1}} Get-Process {{1}} | Out-Null"
     },
     {
       "line": 11,
       "severity": "Error",
       "statement": "Invoke-WebRequest -Uri \"https://logstash.company.com/ingest?u=$username&amp;p=$password\"",
-      "reason": "Sensitive variable `$password` is being sent over HTTP to an external service.",
-      "recommendation": "Use HTTPS instead of HTTP, and consider using more secure authentication methods like API keys or tokens instead of passwords in URLs.",
-      "code_suggestion": "Invoke-WebRequest -Uri \"https://logstash.company.com/ingest?u=$username&amp;p=$password\" -UseBasicParsing"
+      "reason": "Sensitive variable `$password` is being transmitted over the network in plain text.",
+      "recommendation": "Use HTTPS and consider encrypting or hashing sensitive data before transmission.",
+      "code_suggestion": "Invoke-WebRequest -Uri \"https://logstash.company.com/ingest?u=$username&amp;p=$(ConvertTo-SecureString $password -AsPlainText -Force)\""
     },
     {
       "line": 13,
       "severity": "Error",
       "statement": "Set-Content -Path \"C:\\temp\\session_info.txt\" -Value \"User=$username Password=$password Host=$remoteHost\"",
       "reason": "Sensitive variable `$password` is being written to a file in plain text.",
-      "recommendation": "Never store passwords or other sensitive credentials in files, especially not in plain text. Use secure storage solutions like password vaults or encrypted configuration files instead.",
+      "recommendation": "Remove this output statement or use a secure method to store session information.",
       "code_suggestion": "Set-Content -Path \"C:\\temp\\session_info.txt\" -Value \"User=$username Host=$remoteHost\""
     }
   ]

</xml_diff>